<commit_message>
Switch back to destop machine.
</commit_message>
<xml_diff>
--- a/OPIDChecks/Uploads/Research 31-May-2019-0241.xlsx
+++ b/OPIDChecks/Uploads/Research 31-May-2019-0241.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apricot\OPID\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCB0ED25-CBB6-4AF2-9ECE-2BF50AB87AC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0AE4FE-1401-49F1-8A68-F00B25B37BA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2010" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="1920" yWindow="852" windowWidth="18864" windowHeight="12108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Research 31-May-2019-0241" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t xml:space="preserve"> Record ID</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Interview Record ID</t>
   </si>
   <si>
@@ -263,12 +260,15 @@
   </si>
   <si>
     <t>Adams, Stephanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RecordID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1108,45 +1108,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43396</v>
       </c>
@@ -1157,19 +1157,19 @@
         <v>298386</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1">
         <v>87403</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43396</v>
       </c>
@@ -1180,19 +1180,19 @@
         <v>298386</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>87402</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42691</v>
       </c>
@@ -1203,19 +1203,19 @@
         <v>272078</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>75107</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42691</v>
       </c>
@@ -1226,19 +1226,19 @@
         <v>272078</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>75109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43235</v>
       </c>
@@ -1249,19 +1249,19 @@
         <v>288836</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1">
         <v>84188</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>42950</v>
       </c>
@@ -1272,19 +1272,19 @@
         <v>279348</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>79777</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43319</v>
       </c>
@@ -1295,19 +1295,19 @@
         <v>295796</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>85805</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43165</v>
       </c>
@@ -1318,16 +1318,16 @@
         <v>286907</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>82900</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43139</v>
       </c>
@@ -1338,19 +1338,19 @@
         <v>286156</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1">
         <v>82419</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43223</v>
       </c>
@@ -1361,19 +1361,19 @@
         <v>288529</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1">
         <v>84004</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>42283</v>
       </c>
@@ -1384,19 +1384,19 @@
         <v>222443</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1">
         <v>67086</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>42943</v>
       </c>
@@ -1407,19 +1407,19 @@
         <v>279105</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1">
         <v>79656</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>42943</v>
       </c>
@@ -1430,19 +1430,19 @@
         <v>279104</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1">
         <v>79656</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>42579</v>
       </c>
@@ -1453,19 +1453,19 @@
         <v>267059</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
         <v>72585</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>42810</v>
       </c>
@@ -1476,19 +1476,19 @@
         <v>275247</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1">
         <v>77179</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>42810</v>
       </c>
@@ -1499,19 +1499,19 @@
         <v>275247</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1">
         <v>77181</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>42969</v>
       </c>
@@ -1522,19 +1522,19 @@
         <v>280040</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1">
         <v>80155</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>42969</v>
       </c>
@@ -1545,19 +1545,19 @@
         <v>280041</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1">
         <v>80155</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43319</v>
       </c>
@@ -1568,19 +1568,19 @@
         <v>295756</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1">
         <v>85777</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43349</v>
       </c>
@@ -1591,16 +1591,16 @@
         <v>296782</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1">
         <v>86369</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43349</v>
       </c>
@@ -1611,16 +1611,16 @@
         <v>296782</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1">
         <v>86370</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>42542</v>
       </c>
@@ -1631,19 +1631,19 @@
         <v>224276</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
         <v>71817</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43314</v>
       </c>
@@ -1654,19 +1654,19 @@
         <v>295672</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1">
         <v>85737</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43328</v>
       </c>
@@ -1677,19 +1677,19 @@
         <v>296175</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1">
         <v>86040</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>42775</v>
       </c>
@@ -1700,19 +1700,19 @@
         <v>274248</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="1">
         <v>76472</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>42997</v>
       </c>
@@ -1723,16 +1723,16 @@
         <v>280621</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1">
         <v>71256492</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43431</v>
       </c>
@@ -1743,16 +1743,16 @@
         <v>300258</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="1">
         <v>88032</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>42957</v>
       </c>
@@ -1763,19 +1763,19 @@
         <v>279623</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="1">
         <v>79947</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43279</v>
       </c>
@@ -1786,19 +1786,19 @@
         <v>294502</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1">
         <v>85087</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43279</v>
       </c>
@@ -1809,19 +1809,19 @@
         <v>294502</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1">
         <v>85088</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43279</v>
       </c>
@@ -1832,19 +1832,19 @@
         <v>294502</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1">
         <v>85780</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43279</v>
       </c>
@@ -1855,19 +1855,19 @@
         <v>294502</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="1">
         <v>85779</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43263</v>
       </c>
@@ -1878,19 +1878,19 @@
         <v>289724</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="1">
         <v>84709</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43200</v>
       </c>
@@ -1901,19 +1901,19 @@
         <v>287708</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1">
         <v>83454</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>42689</v>
       </c>
@@ -1924,19 +1924,19 @@
         <v>271833</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="1">
         <v>74968</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>42381</v>
       </c>
@@ -1947,19 +1947,19 @@
         <v>223418</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="1">
         <v>68765</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>42381</v>
       </c>
@@ -1970,19 +1970,19 @@
         <v>223418</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1">
         <v>68766</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43354</v>
       </c>
@@ -1993,16 +1993,16 @@
         <v>297016</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="1">
         <v>86506</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>42444</v>
       </c>
@@ -2013,19 +2013,19 @@
         <v>224132</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="1">
         <v>69995</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>42950</v>
       </c>
@@ -2036,19 +2036,19 @@
         <v>279367</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="1">
         <v>79794</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42787</v>
       </c>
@@ -2059,19 +2059,19 @@
         <v>274557</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="1">
         <v>76671</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43405</v>
       </c>
@@ -2082,16 +2082,16 @@
         <v>298722</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="1">
         <v>87652</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43405</v>
       </c>
@@ -2102,16 +2102,16 @@
         <v>298722</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1">
         <v>87653</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42383</v>
       </c>
@@ -2122,19 +2122,19 @@
         <v>223487</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45" s="1">
         <v>68859</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>42719</v>
       </c>
@@ -2145,19 +2145,19 @@
         <v>272921</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E46" s="1">
         <v>75624</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>42390</v>
       </c>
@@ -2168,19 +2168,19 @@
         <v>200712</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1">
         <v>69009</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>43377</v>
       </c>
@@ -2191,19 +2191,19 @@
         <v>297815</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E48" s="1">
         <v>87027</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>43209</v>
       </c>
@@ -2214,19 +2214,19 @@
         <v>288096</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E49" s="1">
         <v>83720</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>42955</v>
       </c>
@@ -2237,19 +2237,19 @@
         <v>279528</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" s="1">
         <v>79896</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>42955</v>
       </c>
@@ -2260,19 +2260,19 @@
         <v>279528</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" s="1">
         <v>79897</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>42635</v>
       </c>
@@ -2283,19 +2283,19 @@
         <v>270062</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1">
         <v>73851</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>42773</v>
       </c>
@@ -2306,19 +2306,19 @@
         <v>274103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="1">
         <v>76339</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>42927</v>
       </c>
@@ -2329,19 +2329,19 @@
         <v>278527</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" s="1">
         <v>79320</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>43214</v>
       </c>
@@ -2352,19 +2352,19 @@
         <v>288225</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="1">
         <v>83801</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>42516</v>
       </c>
@@ -2375,19 +2375,19 @@
         <v>217349</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="1">
         <v>71347</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>42516</v>
       </c>
@@ -2398,19 +2398,19 @@
         <v>217349</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="1">
         <v>71348</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>42670</v>
       </c>
@@ -2421,19 +2421,19 @@
         <v>271266</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" s="1">
         <v>74630</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>42670</v>
       </c>
@@ -2444,19 +2444,19 @@
         <v>271266</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E59" s="1">
         <v>74631</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>42899</v>
       </c>
@@ -2467,19 +2467,19 @@
         <v>277737</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" s="1">
         <v>78849</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>42297</v>
       </c>
@@ -2490,19 +2490,19 @@
         <v>204775</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" s="1">
         <v>67399</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>43335</v>
       </c>
@@ -2513,19 +2513,19 @@
         <v>296439</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" s="1">
         <v>86160</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>43123</v>
       </c>
@@ -2536,19 +2536,19 @@
         <v>285537</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" s="1">
         <v>82045</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>43123</v>
       </c>
@@ -2559,19 +2559,19 @@
         <v>285537</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" s="1">
         <v>82046</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>42906</v>
       </c>
@@ -2582,16 +2582,16 @@
         <v>278012</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E65" s="1">
         <v>79000</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>42906</v>
       </c>
@@ -2602,16 +2602,16 @@
         <v>278013</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E66" s="1">
         <v>79000</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>43391</v>
       </c>
@@ -2622,19 +2622,19 @@
         <v>298317</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E67" s="1">
         <v>87362</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>43419</v>
       </c>
@@ -2645,16 +2645,16 @@
         <v>299904</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E68" s="1">
         <v>87863</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>43419</v>
       </c>
@@ -2665,19 +2665,19 @@
         <v>299904</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E69" s="1">
         <v>87864</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>42906</v>
       </c>
@@ -2688,16 +2688,16 @@
         <v>278011</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" s="1">
         <v>79000</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>42950</v>
       </c>
@@ -2708,19 +2708,19 @@
         <v>279356</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E71" s="1">
         <v>79784</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>43305</v>
       </c>
@@ -2731,19 +2731,19 @@
         <v>295232</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E72" s="1">
         <v>85473</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>43405</v>
       </c>
@@ -2754,16 +2754,16 @@
         <v>298719</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1">
         <v>87639</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>43405</v>
       </c>
@@ -2774,16 +2774,16 @@
         <v>298719</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74" s="1">
         <v>87640</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>43419</v>
       </c>
@@ -2794,19 +2794,19 @@
         <v>299907</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E75" s="1">
         <v>87865</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>42591</v>
       </c>
@@ -2817,19 +2817,19 @@
         <v>268971</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E76" s="1">
         <v>73258</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>42402</v>
       </c>
@@ -2840,19 +2840,19 @@
         <v>204772</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E77" s="1">
         <v>69240</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>42402</v>
       </c>
@@ -2863,19 +2863,19 @@
         <v>204772</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E78" s="1">
         <v>69241</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>42801</v>
       </c>
@@ -2886,16 +2886,16 @@
         <v>274976</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E79" s="1">
         <v>76976</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>42801</v>
       </c>
@@ -2906,19 +2906,19 @@
         <v>274976</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E80" s="1">
         <v>76977</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>43256</v>
       </c>
@@ -2929,19 +2929,19 @@
         <v>289410</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E81" s="1">
         <v>84510</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>42544</v>
       </c>
@@ -2952,19 +2952,19 @@
         <v>225189</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E82" s="1">
         <v>71871</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>42544</v>
       </c>
@@ -2975,19 +2975,19 @@
         <v>225189</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E83" s="1">
         <v>71870</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>42565</v>
       </c>
@@ -2998,19 +2998,19 @@
         <v>266877</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E84" s="1">
         <v>72261</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>42997</v>
       </c>
@@ -3021,16 +3021,16 @@
         <v>280656</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E85" s="1">
         <v>396</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>43314</v>
       </c>
@@ -3041,19 +3041,19 @@
         <v>295612</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E86" s="1">
         <v>85684</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>43314</v>
       </c>
@@ -3064,19 +3064,19 @@
         <v>295612</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E87" s="1">
         <v>85683</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>42509</v>
       </c>
@@ -3087,16 +3087,16 @@
         <v>224789</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E88" s="1">
         <v>71146</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch to laptop connection string.
</commit_message>
<xml_diff>
--- a/OPIDChecks/Uploads/Research 31-May-2019-0241.xlsx
+++ b/OPIDChecks/Uploads/Research 31-May-2019-0241.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apricot\OPID\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DCB0ED25-CBB6-4AF2-9ECE-2BF50AB87AC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0AE4FE-1401-49F1-8A68-F00B25B37BA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2010" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="1920" yWindow="852" windowWidth="18864" windowHeight="12108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Research 31-May-2019-0241" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t xml:space="preserve"> Record ID</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Interview Record ID</t>
   </si>
   <si>
@@ -263,12 +260,15 @@
   </si>
   <si>
     <t>Adams, Stephanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RecordID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1108,45 +1108,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43396</v>
       </c>
@@ -1157,19 +1157,19 @@
         <v>298386</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1">
         <v>87403</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43396</v>
       </c>
@@ -1180,19 +1180,19 @@
         <v>298386</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>87402</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42691</v>
       </c>
@@ -1203,19 +1203,19 @@
         <v>272078</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>75107</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42691</v>
       </c>
@@ -1226,19 +1226,19 @@
         <v>272078</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>75109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43235</v>
       </c>
@@ -1249,19 +1249,19 @@
         <v>288836</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1">
         <v>84188</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>42950</v>
       </c>
@@ -1272,19 +1272,19 @@
         <v>279348</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>79777</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43319</v>
       </c>
@@ -1295,19 +1295,19 @@
         <v>295796</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>85805</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43165</v>
       </c>
@@ -1318,16 +1318,16 @@
         <v>286907</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>82900</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43139</v>
       </c>
@@ -1338,19 +1338,19 @@
         <v>286156</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1">
         <v>82419</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43223</v>
       </c>
@@ -1361,19 +1361,19 @@
         <v>288529</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1">
         <v>84004</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>42283</v>
       </c>
@@ -1384,19 +1384,19 @@
         <v>222443</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1">
         <v>67086</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>42943</v>
       </c>
@@ -1407,19 +1407,19 @@
         <v>279105</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1">
         <v>79656</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>42943</v>
       </c>
@@ -1430,19 +1430,19 @@
         <v>279104</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1">
         <v>79656</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>42579</v>
       </c>
@@ -1453,19 +1453,19 @@
         <v>267059</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
         <v>72585</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>42810</v>
       </c>
@@ -1476,19 +1476,19 @@
         <v>275247</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1">
         <v>77179</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>42810</v>
       </c>
@@ -1499,19 +1499,19 @@
         <v>275247</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1">
         <v>77181</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>42969</v>
       </c>
@@ -1522,19 +1522,19 @@
         <v>280040</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1">
         <v>80155</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>42969</v>
       </c>
@@ -1545,19 +1545,19 @@
         <v>280041</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1">
         <v>80155</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43319</v>
       </c>
@@ -1568,19 +1568,19 @@
         <v>295756</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1">
         <v>85777</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43349</v>
       </c>
@@ -1591,16 +1591,16 @@
         <v>296782</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1">
         <v>86369</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43349</v>
       </c>
@@ -1611,16 +1611,16 @@
         <v>296782</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1">
         <v>86370</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>42542</v>
       </c>
@@ -1631,19 +1631,19 @@
         <v>224276</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
         <v>71817</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43314</v>
       </c>
@@ -1654,19 +1654,19 @@
         <v>295672</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1">
         <v>85737</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43328</v>
       </c>
@@ -1677,19 +1677,19 @@
         <v>296175</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1">
         <v>86040</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>42775</v>
       </c>
@@ -1700,19 +1700,19 @@
         <v>274248</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="1">
         <v>76472</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>42997</v>
       </c>
@@ -1723,16 +1723,16 @@
         <v>280621</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1">
         <v>71256492</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43431</v>
       </c>
@@ -1743,16 +1743,16 @@
         <v>300258</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="1">
         <v>88032</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>42957</v>
       </c>
@@ -1763,19 +1763,19 @@
         <v>279623</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="1">
         <v>79947</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43279</v>
       </c>
@@ -1786,19 +1786,19 @@
         <v>294502</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1">
         <v>85087</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43279</v>
       </c>
@@ -1809,19 +1809,19 @@
         <v>294502</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1">
         <v>85088</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43279</v>
       </c>
@@ -1832,19 +1832,19 @@
         <v>294502</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1">
         <v>85780</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43279</v>
       </c>
@@ -1855,19 +1855,19 @@
         <v>294502</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="1">
         <v>85779</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43263</v>
       </c>
@@ -1878,19 +1878,19 @@
         <v>289724</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="1">
         <v>84709</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43200</v>
       </c>
@@ -1901,19 +1901,19 @@
         <v>287708</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1">
         <v>83454</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>42689</v>
       </c>
@@ -1924,19 +1924,19 @@
         <v>271833</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="1">
         <v>74968</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>42381</v>
       </c>
@@ -1947,19 +1947,19 @@
         <v>223418</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="1">
         <v>68765</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>42381</v>
       </c>
@@ -1970,19 +1970,19 @@
         <v>223418</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1">
         <v>68766</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43354</v>
       </c>
@@ -1993,16 +1993,16 @@
         <v>297016</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="1">
         <v>86506</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>42444</v>
       </c>
@@ -2013,19 +2013,19 @@
         <v>224132</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="1">
         <v>69995</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>42950</v>
       </c>
@@ -2036,19 +2036,19 @@
         <v>279367</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="1">
         <v>79794</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42787</v>
       </c>
@@ -2059,19 +2059,19 @@
         <v>274557</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="1">
         <v>76671</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43405</v>
       </c>
@@ -2082,16 +2082,16 @@
         <v>298722</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="1">
         <v>87652</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43405</v>
       </c>
@@ -2102,16 +2102,16 @@
         <v>298722</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1">
         <v>87653</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42383</v>
       </c>
@@ -2122,19 +2122,19 @@
         <v>223487</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45" s="1">
         <v>68859</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>42719</v>
       </c>
@@ -2145,19 +2145,19 @@
         <v>272921</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E46" s="1">
         <v>75624</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>42390</v>
       </c>
@@ -2168,19 +2168,19 @@
         <v>200712</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1">
         <v>69009</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>43377</v>
       </c>
@@ -2191,19 +2191,19 @@
         <v>297815</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E48" s="1">
         <v>87027</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>43209</v>
       </c>
@@ -2214,19 +2214,19 @@
         <v>288096</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E49" s="1">
         <v>83720</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>42955</v>
       </c>
@@ -2237,19 +2237,19 @@
         <v>279528</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" s="1">
         <v>79896</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>42955</v>
       </c>
@@ -2260,19 +2260,19 @@
         <v>279528</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" s="1">
         <v>79897</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>42635</v>
       </c>
@@ -2283,19 +2283,19 @@
         <v>270062</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1">
         <v>73851</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>42773</v>
       </c>
@@ -2306,19 +2306,19 @@
         <v>274103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="1">
         <v>76339</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>42927</v>
       </c>
@@ -2329,19 +2329,19 @@
         <v>278527</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" s="1">
         <v>79320</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>43214</v>
       </c>
@@ -2352,19 +2352,19 @@
         <v>288225</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="1">
         <v>83801</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>42516</v>
       </c>
@@ -2375,19 +2375,19 @@
         <v>217349</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="1">
         <v>71347</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>42516</v>
       </c>
@@ -2398,19 +2398,19 @@
         <v>217349</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="1">
         <v>71348</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>42670</v>
       </c>
@@ -2421,19 +2421,19 @@
         <v>271266</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" s="1">
         <v>74630</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>42670</v>
       </c>
@@ -2444,19 +2444,19 @@
         <v>271266</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E59" s="1">
         <v>74631</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>42899</v>
       </c>
@@ -2467,19 +2467,19 @@
         <v>277737</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" s="1">
         <v>78849</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>42297</v>
       </c>
@@ -2490,19 +2490,19 @@
         <v>204775</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" s="1">
         <v>67399</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>43335</v>
       </c>
@@ -2513,19 +2513,19 @@
         <v>296439</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" s="1">
         <v>86160</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>43123</v>
       </c>
@@ -2536,19 +2536,19 @@
         <v>285537</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" s="1">
         <v>82045</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>43123</v>
       </c>
@@ -2559,19 +2559,19 @@
         <v>285537</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" s="1">
         <v>82046</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>42906</v>
       </c>
@@ -2582,16 +2582,16 @@
         <v>278012</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E65" s="1">
         <v>79000</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>42906</v>
       </c>
@@ -2602,16 +2602,16 @@
         <v>278013</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E66" s="1">
         <v>79000</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>43391</v>
       </c>
@@ -2622,19 +2622,19 @@
         <v>298317</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E67" s="1">
         <v>87362</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>43419</v>
       </c>
@@ -2645,16 +2645,16 @@
         <v>299904</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E68" s="1">
         <v>87863</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>43419</v>
       </c>
@@ -2665,19 +2665,19 @@
         <v>299904</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E69" s="1">
         <v>87864</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>42906</v>
       </c>
@@ -2688,16 +2688,16 @@
         <v>278011</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" s="1">
         <v>79000</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>42950</v>
       </c>
@@ -2708,19 +2708,19 @@
         <v>279356</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E71" s="1">
         <v>79784</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>43305</v>
       </c>
@@ -2731,19 +2731,19 @@
         <v>295232</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E72" s="1">
         <v>85473</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>43405</v>
       </c>
@@ -2754,16 +2754,16 @@
         <v>298719</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1">
         <v>87639</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>43405</v>
       </c>
@@ -2774,16 +2774,16 @@
         <v>298719</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74" s="1">
         <v>87640</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>43419</v>
       </c>
@@ -2794,19 +2794,19 @@
         <v>299907</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E75" s="1">
         <v>87865</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>42591</v>
       </c>
@@ -2817,19 +2817,19 @@
         <v>268971</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E76" s="1">
         <v>73258</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>42402</v>
       </c>
@@ -2840,19 +2840,19 @@
         <v>204772</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E77" s="1">
         <v>69240</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>42402</v>
       </c>
@@ -2863,19 +2863,19 @@
         <v>204772</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E78" s="1">
         <v>69241</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>42801</v>
       </c>
@@ -2886,16 +2886,16 @@
         <v>274976</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E79" s="1">
         <v>76976</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>42801</v>
       </c>
@@ -2906,19 +2906,19 @@
         <v>274976</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E80" s="1">
         <v>76977</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>43256</v>
       </c>
@@ -2929,19 +2929,19 @@
         <v>289410</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E81" s="1">
         <v>84510</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>42544</v>
       </c>
@@ -2952,19 +2952,19 @@
         <v>225189</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E82" s="1">
         <v>71871</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>42544</v>
       </c>
@@ -2975,19 +2975,19 @@
         <v>225189</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E83" s="1">
         <v>71870</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>42565</v>
       </c>
@@ -2998,19 +2998,19 @@
         <v>266877</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E84" s="1">
         <v>72261</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>42997</v>
       </c>
@@ -3021,16 +3021,16 @@
         <v>280656</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E85" s="1">
         <v>396</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>43314</v>
       </c>
@@ -3041,19 +3041,19 @@
         <v>295612</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E86" s="1">
         <v>85684</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>43314</v>
       </c>
@@ -3064,19 +3064,19 @@
         <v>295612</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E87" s="1">
         <v>85683</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>42509</v>
       </c>
@@ -3087,16 +3087,16 @@
         <v>224789</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E88" s="1">
         <v>71146</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>